<commit_message>
Adicionado tratamento automático para aceitar alertas ao finalizar
- Modificada a função `finalizar()`:
  - Aguarda a presença de alertas utilizando `EC.alert_is_present()`.
  - Aceita o alerta automaticamente com `self.driver.switch_to.alert.accept()`.
  - Adicionado log para rastrear sucesso ou falha no processo de aceitação do alerta.

Melhoria no controle de fluxo após o botão Finalizar ser clicado.
</commit_message>
<xml_diff>
--- a/dados_apontamento.xlsx
+++ b/dados_apontamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Fabricio\Trabalho\Ceneged\codigo ceneged\RobosCeneged\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDB62B7-350D-484C-95C8-5514763AAAC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047CB576-9FA5-4344-AEA2-4265C1B339EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5BB472D8-36E3-4281-8C0A-29D75B4D5DA0}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +624,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="K4" s="2">
-        <v>3006940</v>
+        <v>3006950</v>
       </c>
       <c r="L4" s="2">
         <v>2</v>

</xml_diff>